<commit_message>
Dejado a medias el docx de los casos nuevos. Falta poco para acabarlo. También se ha hecho el docx con las eficiencias máximas
</commit_message>
<xml_diff>
--- a/Proyecto/Eficiencias máximas 1-4.xlsx
+++ b/Proyecto/Eficiencias máximas 1-4.xlsx
@@ -402,7 +402,7 @@
   <dimension ref="D1:AP119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Z67" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AM94" sqref="AM94:AM98"/>
+      <selection activeCell="AM94" sqref="AM94:AN98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -973,14 +973,8 @@
       </c>
     </row>
     <row r="9" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ9" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK9" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="2"/>
       <c r="AM9" s="2">
         <f t="shared" si="2"/>
         <v>46.165215885512112</v>
@@ -991,14 +985,9 @@
       </c>
     </row>
     <row r="10" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ10" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK10" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="2"/>
+      <c r="AN10" s="2"/>
     </row>
     <row r="11" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D11" s="1">
@@ -1099,6 +1088,7 @@
         <f t="shared" si="1"/>
         <v>9.0641499965427488E-2</v>
       </c>
+      <c r="AN11" s="2"/>
     </row>
     <row r="12" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D12" s="1">
@@ -1199,6 +1189,7 @@
         <f t="shared" si="1"/>
         <v>0.31061540334453264</v>
       </c>
+      <c r="AN12" s="2"/>
     </row>
     <row r="13" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D13" s="1">
@@ -1299,6 +1290,7 @@
         <f t="shared" si="1"/>
         <v>1.0734344990108238</v>
       </c>
+      <c r="AN13" s="2"/>
     </row>
     <row r="14" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D14" s="1">
@@ -1399,6 +1391,7 @@
         <f t="shared" si="1"/>
         <v>3.7216152032220799</v>
       </c>
+      <c r="AN14" s="2"/>
     </row>
     <row r="15" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D15" s="1">
@@ -1499,28 +1492,19 @@
         <f t="shared" si="1"/>
         <v>7.5022271665818057</v>
       </c>
+      <c r="AN15" s="2"/>
     </row>
     <row r="16" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ16" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK16" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="AJ17" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK17" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="4:37" x14ac:dyDescent="0.25">
+      <c r="AJ16" s="2"/>
+      <c r="AK16" s="2"/>
+      <c r="AN16" s="2"/>
+    </row>
+    <row r="17" spans="4:40" x14ac:dyDescent="0.25">
+      <c r="AJ17" s="2"/>
+      <c r="AK17" s="2"/>
+      <c r="AN17" s="2"/>
+    </row>
+    <row r="18" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D18" s="1">
         <v>1.7335373679600401</v>
       </c>
@@ -1619,8 +1603,9 @@
         <f t="shared" si="1"/>
         <v>5.0706869381540856E-2</v>
       </c>
-    </row>
-    <row r="19" spans="4:37" x14ac:dyDescent="0.25">
+      <c r="AN18" s="2"/>
+    </row>
+    <row r="19" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D19" s="1">
         <v>4.0537131006699099</v>
       </c>
@@ -1719,8 +1704,9 @@
         <f t="shared" si="1"/>
         <v>0.18124352271267188</v>
       </c>
-    </row>
-    <row r="20" spans="4:37" x14ac:dyDescent="0.25">
+      <c r="AN19" s="2"/>
+    </row>
+    <row r="20" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D20" s="1">
         <v>8.8747040372439798</v>
       </c>
@@ -1819,8 +1805,9 @@
         <f t="shared" si="1"/>
         <v>1.0443082531834644</v>
       </c>
-    </row>
-    <row r="21" spans="4:37" x14ac:dyDescent="0.25">
+      <c r="AN20" s="2"/>
+    </row>
+    <row r="21" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D21" s="1">
         <v>20.959522377494899</v>
       </c>
@@ -1919,8 +1906,9 @@
         <f t="shared" si="1"/>
         <v>3.3205822072500424</v>
       </c>
-    </row>
-    <row r="22" spans="4:37" x14ac:dyDescent="0.25">
+      <c r="AN21" s="2"/>
+    </row>
+    <row r="22" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D22" s="1">
         <v>37.824348687319997</v>
       </c>
@@ -2019,28 +2007,19 @@
         <f t="shared" si="1"/>
         <v>9.1322600276730608</v>
       </c>
-    </row>
-    <row r="23" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="AJ23" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK23" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="24" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="AJ24" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK24" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="25" spans="4:37" x14ac:dyDescent="0.25">
+      <c r="AN22" s="2"/>
+    </row>
+    <row r="23" spans="4:40" x14ac:dyDescent="0.25">
+      <c r="AJ23" s="2"/>
+      <c r="AK23" s="2"/>
+      <c r="AN23" s="2"/>
+    </row>
+    <row r="24" spans="4:40" x14ac:dyDescent="0.25">
+      <c r="AJ24" s="2"/>
+      <c r="AK24" s="2"/>
+      <c r="AN24" s="2"/>
+    </row>
+    <row r="25" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D25" s="1">
         <v>1.8753878995876201</v>
       </c>
@@ -2139,8 +2118,9 @@
         <f t="shared" si="1"/>
         <v>9.8903363365453384E-2</v>
       </c>
-    </row>
-    <row r="26" spans="4:37" x14ac:dyDescent="0.25">
+      <c r="AN25" s="2"/>
+    </row>
+    <row r="26" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D26" s="1">
         <v>3.7643305575765398</v>
       </c>
@@ -2239,8 +2219,9 @@
         <f t="shared" si="1"/>
         <v>0.30418311750620536</v>
       </c>
-    </row>
-    <row r="27" spans="4:37" x14ac:dyDescent="0.25">
+      <c r="AN26" s="2"/>
+    </row>
+    <row r="27" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D27" s="1">
         <v>9.9027094080209093</v>
       </c>
@@ -2339,8 +2320,9 @@
         <f t="shared" si="1"/>
         <v>1.119340253315227</v>
       </c>
-    </row>
-    <row r="28" spans="4:37" x14ac:dyDescent="0.25">
+      <c r="AN27" s="2"/>
+    </row>
+    <row r="28" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D28" s="1">
         <v>18.885263506375502</v>
       </c>
@@ -2439,8 +2421,9 @@
         <f t="shared" si="1"/>
         <v>6.6406641018305645</v>
       </c>
-    </row>
-    <row r="29" spans="4:37" x14ac:dyDescent="0.25">
+      <c r="AN28" s="2"/>
+    </row>
+    <row r="29" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D29" s="1">
         <v>47.416717388101802</v>
       </c>
@@ -2539,39 +2522,25 @@
         <f t="shared" si="1"/>
         <v>7.4241393281998409</v>
       </c>
-    </row>
-    <row r="30" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="AJ30" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK30" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="31" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="AJ31" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK31" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="32" spans="4:37" x14ac:dyDescent="0.25">
+      <c r="AN29" s="2"/>
+    </row>
+    <row r="30" spans="4:40" x14ac:dyDescent="0.25">
+      <c r="AJ30" s="2"/>
+      <c r="AK30" s="2"/>
+      <c r="AN30" s="2"/>
+    </row>
+    <row r="31" spans="4:40" x14ac:dyDescent="0.25">
+      <c r="AJ31" s="2"/>
+      <c r="AK31" s="2"/>
+      <c r="AN31" s="2"/>
+    </row>
+    <row r="32" spans="4:40" x14ac:dyDescent="0.25">
       <c r="AF32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AJ32" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK32" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ32" s="2"/>
+      <c r="AK32" s="2"/>
+      <c r="AN32" s="2"/>
     </row>
     <row r="33" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D33" s="1">
@@ -2675,6 +2644,7 @@
       <c r="AM33" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="AN33" s="2"/>
     </row>
     <row r="34" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D34" s="1">
@@ -2779,9 +2749,9 @@
         <f>AVERAGE(AJ33,AJ40,AJ47,AJ54)</f>
         <v>1.8166174848613776</v>
       </c>
-      <c r="AN34" s="2" t="e">
-        <f>_xlfn.STDEV.S(D33:AG33,#REF!,#REF!,D54:AG54)</f>
-        <v>#REF!</v>
+      <c r="AN34" s="2">
+        <f t="shared" ref="AN10:AN34" si="3">_xlfn.STDEV.S(D33:AG33,D40:AG40,D47:AG47,D54:AG54)</f>
+        <v>6.4079087391012687E-2</v>
       </c>
     </row>
     <row r="35" spans="4:40" x14ac:dyDescent="0.25">
@@ -2884,7 +2854,7 @@
         <v>0.7015904707751317</v>
       </c>
       <c r="AM35" s="2">
-        <f t="shared" ref="AM35:AM37" si="3">AVERAGE(AJ34,AJ41,AJ48,AJ55)</f>
+        <f t="shared" ref="AM35:AM37" si="4">AVERAGE(AJ34,AJ41,AJ48,AJ55)</f>
         <v>4.3756918553179478</v>
       </c>
       <c r="AN35" s="2">
@@ -2992,7 +2962,7 @@
         <v>3.2462850167849049</v>
       </c>
       <c r="AM36" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.6303406481108027</v>
       </c>
       <c r="AN36" s="2">
@@ -3100,7 +3070,7 @@
         <v>9.7798076794829178</v>
       </c>
       <c r="AM37" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>21.431513456268739</v>
       </c>
       <c r="AN37" s="2">
@@ -3109,14 +3079,8 @@
       </c>
     </row>
     <row r="38" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ38" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK38" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ38" s="2"/>
+      <c r="AK38" s="2"/>
       <c r="AM38" s="2">
         <f>AVERAGE(AJ37,AJ44,AJ51,AJ58)</f>
         <v>57.447113217727598</v>
@@ -3127,14 +3091,8 @@
       </c>
     </row>
     <row r="39" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ39" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK39" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ39" s="2"/>
+      <c r="AK39" s="2"/>
     </row>
     <row r="40" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D40" s="1">
@@ -3637,24 +3595,12 @@
       </c>
     </row>
     <row r="45" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ45" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK45" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ45" s="2"/>
+      <c r="AK45" s="2"/>
     </row>
     <row r="46" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ46" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK46" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ46" s="2"/>
+      <c r="AK46" s="2"/>
     </row>
     <row r="47" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D47" s="1">
@@ -4157,24 +4103,12 @@
       </c>
     </row>
     <row r="52" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ52" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK52" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ52" s="2"/>
+      <c r="AK52" s="2"/>
     </row>
     <row r="53" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ53" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK53" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ53" s="2"/>
+      <c r="AK53" s="2"/>
     </row>
     <row r="54" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D54" s="1">
@@ -4677,47 +4611,23 @@
       </c>
     </row>
     <row r="59" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ59" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK59" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ59" s="2"/>
+      <c r="AK59" s="2"/>
     </row>
     <row r="60" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ60" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK60" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ60" s="2"/>
+      <c r="AK60" s="2"/>
     </row>
     <row r="61" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ61" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK61" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ61" s="2"/>
+      <c r="AK61" s="2"/>
     </row>
     <row r="62" spans="4:40" x14ac:dyDescent="0.25">
       <c r="AF62" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AJ62" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK62" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ62" s="2"/>
+      <c r="AK62" s="2"/>
     </row>
     <row r="63" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D63" s="1">
@@ -5030,7 +4940,7 @@
         <v>6.8790083692925119</v>
       </c>
       <c r="AM65" s="2">
-        <f t="shared" ref="AM65:AM68" si="4">AVERAGE(AJ64,AJ71,AJ78,AJ85)</f>
+        <f t="shared" ref="AM65:AM68" si="5">AVERAGE(AJ64,AJ71,AJ78,AJ85)</f>
         <v>12.052589142255759</v>
       </c>
       <c r="AN65" s="2">
@@ -5138,7 +5048,7 @@
         <v>11.823405404889506</v>
       </c>
       <c r="AM66" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>27.984393436998417</v>
       </c>
       <c r="AN66" s="2">
@@ -5246,7 +5156,7 @@
         <v>30.012618203056519</v>
       </c>
       <c r="AM67" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>57.092811559663716</v>
       </c>
       <c r="AN67" s="2">
@@ -5255,16 +5165,10 @@
       </c>
     </row>
     <row r="68" spans="4:42" x14ac:dyDescent="0.25">
-      <c r="AJ68" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK68" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ68" s="2"/>
+      <c r="AK68" s="2"/>
       <c r="AM68" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>144.45257041170015</v>
       </c>
       <c r="AN68" s="2">
@@ -5273,14 +5177,8 @@
       </c>
     </row>
     <row r="69" spans="4:42" x14ac:dyDescent="0.25">
-      <c r="AJ69" s="2" t="e">
-        <f t="shared" ref="AJ69:AJ118" si="5">AVERAGE(D69:AG69)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK69" s="2" t="e">
-        <f t="shared" ref="AK69:AK118" si="6">_xlfn.STDEV.S(D69:AG69)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ69" s="2"/>
+      <c r="AK69" s="2"/>
     </row>
     <row r="70" spans="4:42" x14ac:dyDescent="0.25">
       <c r="D70" s="1">
@@ -5374,11 +5272,11 @@
         <v>1.87747010962299</v>
       </c>
       <c r="AJ70" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="AJ69:AJ118" si="6">AVERAGE(D70:AG70)</f>
         <v>2.9893244013341205</v>
       </c>
       <c r="AK70" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="AK69:AK118" si="7">_xlfn.STDEV.S(D70:AG70)</f>
         <v>1.1075742881402475</v>
       </c>
     </row>
@@ -5474,11 +5372,11 @@
         <v>15.1344041249646</v>
       </c>
       <c r="AJ71" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12.092107680656881</v>
       </c>
       <c r="AK71" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.1390630783759894</v>
       </c>
     </row>
@@ -5574,11 +5472,11 @@
         <v>37.7384282513569</v>
       </c>
       <c r="AJ72" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>28.87191849164331</v>
       </c>
       <c r="AK72" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.7264987487393642</v>
       </c>
     </row>
@@ -5674,11 +5572,11 @@
         <v>51.832911265547402</v>
       </c>
       <c r="AJ73" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>55.65056021501799</v>
       </c>
       <c r="AK73" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12.222108234021499</v>
       </c>
     </row>
@@ -5774,33 +5672,21 @@
         <v>239.181796528522</v>
       </c>
       <c r="AJ74" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>147.97148894803135</v>
       </c>
       <c r="AK74" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>36.674950325095843</v>
       </c>
     </row>
     <row r="75" spans="4:42" x14ac:dyDescent="0.25">
-      <c r="AJ75" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK75" s="2" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ75" s="2"/>
+      <c r="AK75" s="2"/>
     </row>
     <row r="76" spans="4:42" x14ac:dyDescent="0.25">
-      <c r="AJ76" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK76" s="2" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ76" s="2"/>
+      <c r="AK76" s="2"/>
       <c r="AO76" s="2"/>
       <c r="AP76" s="4"/>
     </row>
@@ -5896,11 +5782,11 @@
         <v>1.8943814716784699</v>
       </c>
       <c r="AJ77" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.9746611593195587</v>
       </c>
       <c r="AK77" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0213357418720868</v>
       </c>
       <c r="AO77" s="2"/>
@@ -5998,11 +5884,11 @@
         <v>15.194503047151899</v>
       </c>
       <c r="AJ78" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12.061440348962808</v>
       </c>
       <c r="AK78" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.0353273319794196</v>
       </c>
       <c r="AO78" s="2"/>
@@ -6100,11 +5986,11 @@
         <v>29.225280924675701</v>
       </c>
       <c r="AJ79" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>27.059581837451635</v>
       </c>
       <c r="AK79" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.9381889467367523</v>
       </c>
     </row>
@@ -6200,11 +6086,11 @@
         <v>51.585024819602701</v>
       </c>
       <c r="AJ80" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>59.150538620215109</v>
       </c>
       <c r="AK80" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>15.544716771594752</v>
       </c>
     </row>
@@ -6300,33 +6186,21 @@
         <v>135.006961840521</v>
       </c>
       <c r="AJ81" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>143.74672376631256</v>
       </c>
       <c r="AK81" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>34.469903603986197</v>
       </c>
     </row>
     <row r="82" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ82" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK82" s="2" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ82" s="2"/>
+      <c r="AK82" s="2"/>
     </row>
     <row r="83" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ83" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK83" s="2" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ83" s="2"/>
+      <c r="AK83" s="2"/>
     </row>
     <row r="84" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D84" s="1">
@@ -6420,11 +6294,11 @@
         <v>1.8717648702080101</v>
       </c>
       <c r="AJ84" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.0127802534972932</v>
       </c>
       <c r="AK84" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1337111241331668</v>
       </c>
     </row>
@@ -6520,11 +6394,11 @@
         <v>14.0589579192028</v>
       </c>
       <c r="AJ85" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12.063496085572293</v>
       </c>
       <c r="AK85" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.049570083497942</v>
       </c>
     </row>
@@ -6620,11 +6494,11 @@
         <v>32.630795027874299</v>
       </c>
       <c r="AJ86" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>28.115746628701309</v>
       </c>
       <c r="AK86" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.9401911576444988</v>
       </c>
     </row>
@@ -6720,11 +6594,11 @@
         <v>36.747193243703897</v>
       </c>
       <c r="AJ87" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>56.527110907566239</v>
       </c>
       <c r="AK87" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13.774878034530461</v>
       </c>
     </row>
@@ -6820,56 +6694,32 @@
         <v>129.65052573481401</v>
       </c>
       <c r="AJ88" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>143.51382274379148</v>
       </c>
       <c r="AK88" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>35.592550086673555</v>
       </c>
     </row>
     <row r="89" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ89" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK89" s="2" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ89" s="2"/>
+      <c r="AK89" s="2"/>
     </row>
     <row r="90" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ90" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK90" s="2" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ90" s="2"/>
+      <c r="AK90" s="2"/>
     </row>
     <row r="91" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ91" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK91" s="2" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ91" s="2"/>
+      <c r="AK91" s="2"/>
     </row>
     <row r="92" spans="4:40" x14ac:dyDescent="0.25">
       <c r="AF92" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AJ92" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK92" s="2" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ92" s="2"/>
+      <c r="AK92" s="2"/>
     </row>
     <row r="93" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D93" s="1">
@@ -6963,11 +6813,11 @@
         <v>4.0253865571121796</v>
       </c>
       <c r="AJ93" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.9208515431010635</v>
       </c>
       <c r="AK93" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.98262761810157395</v>
       </c>
       <c r="AM93" s="1" t="s">
@@ -7066,11 +6916,11 @@
         <v>14.0059916930732</v>
       </c>
       <c r="AJ94" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10.803107803725172</v>
       </c>
       <c r="AK94" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.1945751337292569</v>
       </c>
       <c r="AM94" s="2">
@@ -7174,15 +7024,15 @@
         <v>33.645884513271099</v>
       </c>
       <c r="AJ95" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>26.455048628443695</v>
       </c>
       <c r="AK95" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.2820484166911177</v>
       </c>
       <c r="AM95" s="2">
-        <f t="shared" ref="AM95:AM98" si="7">AVERAGE(AJ94,AJ101,AJ108,AJ115)</f>
+        <f t="shared" ref="AM95:AM98" si="8">AVERAGE(AJ94,AJ101,AJ108,AJ115)</f>
         <v>10.937666684704672</v>
       </c>
       <c r="AN95" s="2">
@@ -7282,11 +7132,11 @@
         <v>80.821155779112203</v>
       </c>
       <c r="AJ96" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>64.561916228057356</v>
       </c>
       <c r="AK96" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>16.105053923607247</v>
       </c>
       <c r="AM96" s="2">
@@ -7390,15 +7240,15 @@
         <v>205.24172226536501</v>
       </c>
       <c r="AJ97" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>179.82494412186404</v>
       </c>
       <c r="AK97" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>50.645839362420844</v>
       </c>
       <c r="AM97" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>61.016029252835921</v>
       </c>
       <c r="AN97" s="2">
@@ -7407,16 +7257,10 @@
       </c>
     </row>
     <row r="98" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ98" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK98" s="2" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ98" s="2"/>
+      <c r="AK98" s="2"/>
       <c r="AM98" s="2">
-        <f t="shared" si="7"/>
+        <f>AVERAGE(AJ97,AJ104,AJ111,AJ118)</f>
         <v>170.00332855406748</v>
       </c>
       <c r="AN98" s="2">
@@ -7425,14 +7269,8 @@
       </c>
     </row>
     <row r="99" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ99" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK99" s="2" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ99" s="2"/>
+      <c r="AK99" s="2"/>
     </row>
     <row r="100" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D100" s="1">
@@ -7526,11 +7364,11 @@
         <v>4.0130518871439396</v>
       </c>
       <c r="AJ100" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.8919553271283478</v>
       </c>
       <c r="AK100" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.95704096113637915</v>
       </c>
     </row>
@@ -7626,11 +7464,11 @@
         <v>13.2313758973497</v>
       </c>
       <c r="AJ101" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11.139285430464545</v>
       </c>
       <c r="AK101" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.3288299516284705</v>
       </c>
     </row>
@@ -7726,11 +7564,11 @@
         <v>26.870219953197999</v>
       </c>
       <c r="AJ102" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>27.36689022258436</v>
       </c>
       <c r="AK102" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.7369694078232145</v>
       </c>
     </row>
@@ -7826,11 +7664,11 @@
         <v>55.055946363329802</v>
       </c>
       <c r="AJ103" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>58.667200210032327</v>
       </c>
       <c r="AK103" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>15.851284338516974</v>
       </c>
     </row>
@@ -7926,33 +7764,21 @@
         <v>237.94145741111001</v>
       </c>
       <c r="AJ104" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>167.86248535138523</v>
       </c>
       <c r="AK104" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>34.90307623659988</v>
       </c>
     </row>
     <row r="105" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ105" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK105" s="2" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ105" s="2"/>
+      <c r="AK105" s="2"/>
     </row>
     <row r="106" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ106" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK106" s="2" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ106" s="2"/>
+      <c r="AK106" s="2"/>
     </row>
     <row r="107" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D107" s="1">
@@ -8046,11 +7872,11 @@
         <v>4.0781657857366902</v>
       </c>
       <c r="AJ107" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.9430174304724606</v>
       </c>
       <c r="AK107" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0092038782511032</v>
       </c>
     </row>
@@ -8146,11 +7972,11 @@
         <v>14.4638227325303</v>
       </c>
       <c r="AJ108" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10.904136752314484</v>
       </c>
       <c r="AK108" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.3858722649711295</v>
       </c>
     </row>
@@ -8246,11 +8072,11 @@
         <v>31.304684555454202</v>
       </c>
       <c r="AJ109" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>26.216099478426219</v>
       </c>
       <c r="AK109" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.3095648102768571</v>
       </c>
     </row>
@@ -8346,11 +8172,11 @@
         <v>66.865923809316598</v>
       </c>
       <c r="AJ110" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>60.417500286627003</v>
       </c>
       <c r="AK110" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11.637672249236589</v>
       </c>
     </row>
@@ -8446,33 +8272,21 @@
         <v>166.199195013847</v>
       </c>
       <c r="AJ111" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>166.1629423715103</v>
       </c>
       <c r="AK111" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39.849774174132939</v>
       </c>
     </row>
     <row r="112" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="AJ112" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK112" s="2" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ112" s="2"/>
+      <c r="AK112" s="2"/>
     </row>
     <row r="113" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="AJ113" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK113" s="2" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AJ113" s="2"/>
+      <c r="AK113" s="2"/>
     </row>
     <row r="114" spans="4:37" x14ac:dyDescent="0.25">
       <c r="D114" s="1">
@@ -8566,11 +8380,11 @@
         <v>4.0781657857366902</v>
       </c>
       <c r="AJ114" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.9430174304724606</v>
       </c>
       <c r="AK114" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0092038782511032</v>
       </c>
     </row>
@@ -8666,11 +8480,11 @@
         <v>14.4638227325303</v>
       </c>
       <c r="AJ115" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10.904136752314484</v>
       </c>
       <c r="AK115" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.3858722649711295</v>
       </c>
     </row>
@@ -8766,11 +8580,11 @@
         <v>31.304684555454202</v>
       </c>
       <c r="AJ116" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>26.216099478426219</v>
       </c>
       <c r="AK116" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.3095648102768571</v>
       </c>
     </row>
@@ -8866,11 +8680,11 @@
         <v>66.865923809316598</v>
       </c>
       <c r="AJ117" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>60.417500286627003</v>
       </c>
       <c r="AK117" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11.637672249236589</v>
       </c>
     </row>
@@ -8966,11 +8780,11 @@
         <v>166.199195013847</v>
       </c>
       <c r="AJ118" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>166.1629423715103</v>
       </c>
       <c r="AK118" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39.849774174132939</v>
       </c>
     </row>

</xml_diff>